<commit_message>
add logger + feature 28/5
</commit_message>
<xml_diff>
--- a/data/Địa-chỉ.xlsx
+++ b/data/Địa-chỉ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damtr\PycharmProjects\api_phone_address\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E8C73B-52AB-4612-B961-FA12780D6102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C766CF-7D63-4821-BF75-527544ABD18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7F5B9479-D054-445F-B4FF-C1FB3E6E2895}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Xã an hiệp.  Khu công nghiệp an hiệp. Huyện châu thành.  Tỉnh bến tre</t>
   </si>
@@ -302,6 +302,19 @@
   </si>
   <si>
     <t>Em o xa vinh thanh aq vinh to</t>
+  </si>
+  <si>
+    <t>Cây số 1 giá bao nhiêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia chj bunkbu xa hoa khah , tp buon ma thuot đaklak , sdt 0369333915 , ten bia
+</t>
+  </si>
+  <si>
+    <t>Tôi muốn lấy thêm 02 bao thì giá bao nhiêu</t>
+  </si>
+  <si>
+    <t>Chiều dài con dao bao nhiêu vậy bạn</t>
   </si>
 </sst>
 </file>
@@ -706,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BBEB7F-A291-4C2F-B7EC-267C92C74EE6}">
-  <dimension ref="A1:A84"/>
+  <dimension ref="A1:A88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,6 +1150,26 @@
         <v>83</v>
       </c>
     </row>
+    <row r="85" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>